<commit_message>
Fixing RAD Test Cases and Data
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EmailNoMatch.xlsx
+++ b/KatalonData/RADTestData/EmailNoMatch.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="79">
   <si>
     <t>Execute</t>
   </si>
@@ -253,6 +253,24 @@
   </si>
   <si>
     <t>Fri Nov 19 10:49:30 EST 2021</t>
+  </si>
+  <si>
+    <t>Thu Oct 20 21:34:11 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 20 21:34:20 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 20 21:34:27 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 20 21:34:33 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 20 21:34:39 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 20 21:34:46 EDT 2022</t>
   </si>
 </sst>
 </file>
@@ -638,7 +656,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -652,7 +670,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -666,7 +684,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -680,7 +698,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -694,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -708,7 +726,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added EL-NumberValidation Test Case and Data.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EmailNoMatch.xlsx
+++ b/KatalonData/RADTestData/EmailNoMatch.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="85">
   <si>
     <t>Execute</t>
   </si>
@@ -271,6 +271,24 @@
   </si>
   <si>
     <t>Thu Oct 20 21:34:46 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Nov 02 16:23:34 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Nov 02 16:23:46 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Nov 02 16:23:56 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Nov 02 16:24:07 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Nov 02 16:24:17 EDT 2022</t>
+  </si>
+  <si>
+    <t>Wed Nov 02 16:24:28 EDT 2022</t>
   </si>
 </sst>
 </file>
@@ -656,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -670,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -684,7 +702,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -698,7 +716,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -712,7 +730,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -726,7 +744,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added and updated Negative Test Cases for RAD.
</commit_message>
<xml_diff>
--- a/KatalonData/RADTestData/EmailNoMatch.xlsx
+++ b/KatalonData/RADTestData/EmailNoMatch.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3BFC66F0-0B55-4D16-B9D6-6829D2ACE823}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9801522A-FB83-4ADF-B687-DD718FE1CB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17640" windowWidth="29040" xWindow="-28920" xr2:uid="{8832F8CD-C84D-4F68-8EAE-C2E28DFA491F}" yWindow="-120"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8832F8CD-C84D-4F68-8EAE-C2E28DFA491F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Execute</t>
   </si>
@@ -51,77 +51,34 @@
     <t>Estimated Tax</t>
   </si>
   <si>
-    <t>Personal Income Tax</t>
-  </si>
-  <si>
     <t>Extension Payments</t>
   </si>
   <si>
     <t>Existing Liability</t>
   </si>
   <si>
-    <t>Sales and Use</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Sun Jul 16 12:08:45 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Jul 16 12:08:55 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Jul 16 12:09:04 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Jul 16 12:09:14 EDT 2023</t>
-  </si>
-  <si>
-    <t>Sun Jul 16 12:09:23 EDT 2023</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Mon Jul 17 19:18:38 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 19:18:47 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 19:18:57 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 19:19:06 EDT 2023</t>
-  </si>
-  <si>
-    <t>Mon Jul 17 19:19:16 EDT 2023</t>
-  </si>
-  <si>
     <t>Mon Jul 17 21:10:59 EDT 2023</t>
   </si>
   <si>
-    <t>Mon Jul 17 21:11:08 EDT 2023</t>
-  </si>
-  <si>
     <t>Mon Jul 17 21:11:18 EDT 2023</t>
   </si>
   <si>
     <t>Mon Jul 17 21:11:27 EDT 2023</t>
   </si>
   <si>
-    <t>Mon Jul 17 21:11:37 EDT 2023</t>
+    <t>New Liability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,16 +106,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -175,10 +132,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -213,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -265,7 +222,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -376,21 +333,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -407,7 +364,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -459,26 +416,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2750B36-BDE9-40E0-AADF-384378C45A8A}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2750B36-BDE9-40E0-AADF-384378C45A8A}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,13 +454,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -511,13 +468,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -525,49 +482,29 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>

</xml_diff>